<commit_message>
antes de los correos
</commit_message>
<xml_diff>
--- a/proveedores_correos.xlsx
+++ b/proveedores_correos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\comprobantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9BC5AC-53CF-45F6-AD63-ABAFD20D7D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A3D18D-F18F-45A2-B74B-7AEC0B026C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="365">
   <si>
     <t>NIT</t>
   </si>
@@ -565,6 +565,15 @@
     <t>AZULK</t>
   </si>
   <si>
+    <t>ORF S.A</t>
+  </si>
+  <si>
+    <t>TECNOQUIMICAS S.A</t>
+  </si>
+  <si>
+    <t>Sokuciones Mana s.a.s</t>
+  </si>
+  <si>
     <t>AREPASRIONEGRO@HOTMAIL.COM</t>
   </si>
   <si>
@@ -1097,13 +1106,22 @@
   </si>
   <si>
     <t>YANETH.SUAREZ@AZULK.COM</t>
+  </si>
+  <si>
+    <t>vmontoya@orf.com.co</t>
+  </si>
+  <si>
+    <t>evillegasa@tqgrupo.com</t>
+  </si>
+  <si>
+    <t>Ventas@freezen.com.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1127,8 +1145,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1138,6 +1164,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAD1DC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA4335"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1317,21 +1385,6 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFF8F9FA"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFF8F9FA"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF442F65"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
@@ -1420,108 +1473,131 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1824,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,1124 +1928,1124 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="22">
         <v>70723847</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="23">
         <v>900177158</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="23">
         <v>900292365</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="23">
         <v>900489731</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="23">
         <v>900310263</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="23">
         <v>900940223</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="23">
         <v>901673248</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="23">
         <v>900842621</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="23">
         <v>800229063</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="23">
         <v>900247844</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12" s="23">
         <v>1040732318</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13" s="23">
         <v>98490086</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="23">
         <v>71385168</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15" s="23">
         <v>900050934</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16" s="23">
         <v>830006735</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17" s="23">
         <v>830006735</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18" s="23">
         <v>830002366</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19" s="23">
         <v>900225463</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20" s="23">
         <v>900407316</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="A21" s="23">
         <v>811011302</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22" s="23">
         <v>890315540</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="A23" s="23">
         <v>892301290</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="A24" s="23">
         <v>800102638</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
+      <c r="A25" s="23">
         <v>800156889</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="A26" s="23">
         <v>900269388</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+      <c r="A27" s="23">
         <v>901526838</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
+      <c r="A28" s="23">
         <v>901605653</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+      <c r="A29" s="23">
         <v>900080654</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
+      <c r="A30" s="23">
         <v>900090524</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+      <c r="A31" s="23">
         <v>830050346</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+      <c r="A32" s="23">
         <v>901371573</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="B32" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
+      <c r="A33" s="23">
         <v>900467903</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34" s="23">
         <v>901352950</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+      <c r="A35" s="23">
         <v>901981258</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
+      <c r="A36" s="23">
         <v>890304130</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+      <c r="A37" s="23">
         <v>901237665</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+      <c r="A38" s="23">
         <v>901476943</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="B38" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
+      <c r="A39" s="23">
         <v>890938750</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="B39" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5">
+      <c r="A40" s="23">
         <v>901040688</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C40" s="6" t="s">
+      <c r="B40" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7">
+      <c r="A41" s="24">
         <v>714800505</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="C41" s="8" t="s">
+      <c r="B41" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
+      <c r="A42" s="23">
         <v>900438907</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="B42" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5">
+      <c r="A43" s="23">
         <v>890900943</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="B43" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+      <c r="A44" s="23">
         <v>890900943</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C44" s="6" t="s">
+      <c r="B44" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5">
+      <c r="A45" s="23">
         <v>890900943</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="B45" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
+      <c r="A46" s="23">
         <v>890911625</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C46" s="6" t="s">
+      <c r="B46" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5">
+      <c r="A47" s="23">
         <v>1034986275</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C47" s="6" t="s">
+      <c r="B47" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="5">
+      <c r="A48" s="23">
         <v>900839722</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C48" s="6" t="s">
+      <c r="B48" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="5">
+      <c r="A49" s="23">
         <v>890700058</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C49" s="6" t="s">
+      <c r="B49" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="9">
+      <c r="A50" s="25">
         <v>860002130</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="C50" s="10" t="s">
+      <c r="B50" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9">
+      <c r="A51" s="25">
         <v>860002130</v>
       </c>
-      <c r="B51" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="C51" s="10" t="s">
+      <c r="B51" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="9">
+      <c r="A52" s="25">
         <v>811012769</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="C52" s="10" t="s">
+      <c r="B52" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="9">
+      <c r="A53" s="25">
         <v>80220499</v>
       </c>
-      <c r="B53" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="C53" s="10" t="s">
+      <c r="B53" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9">
+      <c r="A54" s="25">
         <v>800240674</v>
       </c>
-      <c r="B54" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C54" s="10" t="s">
+      <c r="B54" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="9">
+      <c r="A55" s="25">
         <v>800240674</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C55" s="10" t="s">
+      <c r="B55" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="9">
+      <c r="A56" s="25">
         <v>900256457</v>
       </c>
-      <c r="B56" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="C56" s="10" t="s">
+      <c r="B56" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9">
+      <c r="A57" s="25">
         <v>900256457</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="C57" s="10" t="s">
+      <c r="B57" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="9">
+      <c r="A58" s="25">
         <v>891300382</v>
       </c>
-      <c r="B58" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="C58" s="10" t="s">
+      <c r="B58" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="9">
+      <c r="A59" s="25">
         <v>901700063</v>
       </c>
-      <c r="B59" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="C59" s="10" t="s">
+      <c r="B59" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C59" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="9">
+      <c r="A60" s="25">
         <v>860007955</v>
       </c>
-      <c r="B60" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="C60" s="10" t="s">
+      <c r="B60" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="9">
+      <c r="A61" s="25">
         <v>900909162</v>
       </c>
-      <c r="B61" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="C61" s="10" t="s">
+      <c r="B61" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="9">
+      <c r="A62" s="25">
         <v>901360217</v>
       </c>
-      <c r="B62" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="C62" s="11" t="s">
+      <c r="B62" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C62" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="12">
+      <c r="A63" s="26">
         <v>890909192</v>
       </c>
-      <c r="B63" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C63" s="14" t="s">
+      <c r="B63" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C63" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="9">
+      <c r="A64" s="25">
         <v>890700058</v>
       </c>
-      <c r="B64" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="C64" s="10" t="s">
+      <c r="B64" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C64" s="7" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="9">
+      <c r="A65" s="25">
         <v>901846940</v>
       </c>
-      <c r="B65" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="C65" s="10" t="s">
+      <c r="B65" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C65" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="15">
+      <c r="A66" s="27">
         <v>901037615</v>
       </c>
-      <c r="B66" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="C66" s="16" t="s">
+      <c r="B66" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="15">
+      <c r="A67" s="27">
         <v>860074450</v>
       </c>
-      <c r="B67" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="C67" s="16" t="s">
+      <c r="B67" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="15">
+      <c r="A68" s="27">
         <v>860031606</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="C68" s="16" t="s">
+      <c r="B68" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="15">
+      <c r="A69" s="27">
         <v>900255015</v>
       </c>
-      <c r="B69" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="C69" s="16" t="s">
+      <c r="B69" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="15">
+      <c r="A70" s="27">
         <v>811042361</v>
       </c>
-      <c r="B70" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="C70" s="17" t="s">
+      <c r="B70" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C70" s="21" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="18">
+      <c r="A71" s="28">
         <v>800237815</v>
       </c>
-      <c r="B71" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="C71" s="14" t="s">
+      <c r="B71" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C71" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="15">
+      <c r="A72" s="27">
         <v>900217288</v>
       </c>
-      <c r="B72" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="C72" s="16" t="s">
+      <c r="B72" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="15">
+      <c r="A73" s="27">
         <v>900066809</v>
       </c>
-      <c r="B73" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="C73" s="16" t="s">
+      <c r="B73" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="15">
+      <c r="A74" s="27">
         <v>900166251</v>
       </c>
-      <c r="B74" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="C74" s="16" t="s">
+      <c r="B74" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C74" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="15">
+      <c r="A75" s="27">
         <v>901238214</v>
       </c>
-      <c r="B75" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="C75" s="16" t="s">
+      <c r="B75" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="15">
+      <c r="A76" s="27">
         <v>900314952</v>
       </c>
-      <c r="B76" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="C76" s="17" t="s">
+      <c r="B76" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C76" s="21" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="18">
+      <c r="A77" s="28">
         <v>890937015</v>
       </c>
-      <c r="B77" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="C77" s="14" t="s">
+      <c r="B77" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C77" s="20" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="15">
+      <c r="A78" s="27">
         <v>901022272</v>
       </c>
-      <c r="B78" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="C78" s="16" t="s">
+      <c r="B78" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="15">
+      <c r="A79" s="27">
         <v>900314952</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="C79" s="16" t="s">
+      <c r="B79" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="15">
+      <c r="A80" s="27">
         <v>890936374</v>
       </c>
-      <c r="B80" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="C80" s="16" t="s">
+      <c r="B80" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="20">
+      <c r="A81" s="29">
         <v>900341086</v>
       </c>
-      <c r="B81" s="21" t="s">
-        <v>257</v>
-      </c>
-      <c r="C81" s="21" t="s">
+      <c r="B81" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C81" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="9">
+      <c r="A82" s="25">
         <v>901123355</v>
       </c>
-      <c r="B82" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C82" s="10" t="s">
+      <c r="B82" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C82" s="7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="15">
+      <c r="A83" s="27">
         <v>900747086</v>
       </c>
-      <c r="B83" s="16" t="s">
-        <v>259</v>
-      </c>
-      <c r="C83" s="16" t="s">
+      <c r="B83" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="15">
+      <c r="A84" s="27">
         <v>901935919</v>
       </c>
-      <c r="B84" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="C84" s="16" t="s">
+      <c r="B84" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="15">
+      <c r="A85" s="27">
         <v>800200243</v>
       </c>
-      <c r="B85" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="C85" s="16" t="s">
+      <c r="B85" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C85" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="15">
+      <c r="A86" s="27">
         <v>900290826</v>
       </c>
-      <c r="B86" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="C86" s="16" t="s">
+      <c r="B86" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C86" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="15">
+      <c r="A87" s="27">
         <v>901143842</v>
       </c>
-      <c r="B87" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="C87" s="16" t="s">
+      <c r="B87" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C87" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="15">
+      <c r="A88" s="27">
         <v>901352316</v>
       </c>
-      <c r="B88" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="C88" s="16" t="s">
+      <c r="B88" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="15">
+      <c r="A89" s="27">
         <v>900454147</v>
       </c>
-      <c r="B89" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="C89" s="16" t="s">
+      <c r="B89" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="15">
+      <c r="A90" s="27">
         <v>901590426</v>
       </c>
-      <c r="B90" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="C90" s="16" t="s">
+      <c r="B90" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C90" s="9" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="15">
+      <c r="A91" s="27">
         <v>900472077</v>
       </c>
-      <c r="B91" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="C91" s="16" t="s">
+      <c r="B91" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C91" s="9" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="15">
+      <c r="A92" s="27">
         <v>900551889</v>
       </c>
-      <c r="B92" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="C92" s="16" t="s">
+      <c r="B92" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="15">
+      <c r="A93" s="27">
         <v>901406679</v>
       </c>
-      <c r="B93" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="C93" s="16" t="s">
+      <c r="B93" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="15">
+      <c r="A94" s="27">
         <v>811044016</v>
       </c>
-      <c r="B94" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="C94" s="16" t="s">
+      <c r="B94" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C94" s="9" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="15">
+      <c r="A95" s="27">
         <v>900284257</v>
       </c>
-      <c r="B95" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="C95" s="16" t="s">
+      <c r="B95" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C95" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="20">
+      <c r="A96" s="29">
         <v>811035319</v>
       </c>
-      <c r="B96" s="21" t="s">
-        <v>272</v>
-      </c>
-      <c r="C96" s="21" t="s">
+      <c r="B96" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="C96" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="9">
+      <c r="A97" s="25">
         <v>811037075</v>
       </c>
-      <c r="B97" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="C97" s="10" t="s">
+      <c r="B97" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C97" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="9">
+      <c r="A98" s="25">
         <v>901658586</v>
       </c>
-      <c r="B98" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="C98" s="10" t="s">
+      <c r="B98" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C98" s="7" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="9">
+      <c r="A99" s="25">
         <v>890920001</v>
       </c>
-      <c r="B99" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="C99" s="10" t="s">
+      <c r="B99" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C99" s="7" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="9">
+      <c r="A100" s="25">
         <v>890908493</v>
       </c>
-      <c r="B100" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="C100" s="10" t="s">
+      <c r="B100" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C100" s="7" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="9">
+      <c r="A101" s="25">
         <v>890800718</v>
       </c>
-      <c r="B101" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="C101" s="10" t="s">
+      <c r="B101" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C101" s="7" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="9">
+      <c r="A102" s="25">
         <v>800237488</v>
       </c>
-      <c r="B102" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="C102" s="10" t="s">
+      <c r="B102" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C102" s="7" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="9">
+      <c r="A103" s="25">
         <v>900666117</v>
       </c>
-      <c r="B103" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="C103" s="10" t="s">
+      <c r="B103" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C103" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -2977,13 +3053,13 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="9">
+      <c r="A104" s="25">
         <v>800003193</v>
       </c>
-      <c r="B104" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="C104" s="10" t="s">
+      <c r="B104" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C104" s="7" t="s">
         <v>104</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2991,13 +3067,13 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="9">
+      <c r="A105" s="25">
         <v>901125766</v>
       </c>
-      <c r="B105" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C105" s="11" t="s">
+      <c r="B105" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C105" s="19" t="s">
         <v>105</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -3005,938 +3081,961 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="22">
+      <c r="A106" s="30">
         <v>901057595</v>
       </c>
-      <c r="B106" s="23" t="s">
-        <v>282</v>
-      </c>
-      <c r="C106" s="14" t="s">
+      <c r="B106" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C106" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="9">
+      <c r="A107" s="25">
         <v>811016824</v>
       </c>
-      <c r="B107" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="C107" s="10" t="s">
+      <c r="B107" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C107" s="7" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="9">
+      <c r="A108" s="25">
         <v>900835111</v>
       </c>
-      <c r="B108" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="C108" s="10" t="s">
+      <c r="B108" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C108" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="9">
+      <c r="A109" s="25">
         <v>901378950</v>
       </c>
-      <c r="B109" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="C109" s="10" t="s">
+      <c r="B109" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C109" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="9">
+      <c r="A110" s="25">
         <v>800066000</v>
       </c>
-      <c r="B110" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="C110" s="10" t="s">
+      <c r="B110" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C110" s="7" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="9">
+      <c r="A111" s="25">
         <v>900229009</v>
       </c>
-      <c r="B111" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="C111" s="10" t="s">
+      <c r="B111" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C111" s="7" t="s">
         <v>112</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="9">
+    <row r="112" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="25">
         <v>817001532</v>
       </c>
-      <c r="B112" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="C112" s="10" t="s">
+      <c r="B112" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="C112" s="7" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="9">
+      <c r="A113" s="25">
         <v>800243613</v>
       </c>
-      <c r="B113" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="C113" s="10" t="s">
+      <c r="B113" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C113" s="7" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="9">
+      <c r="A114" s="25">
         <v>890934395</v>
       </c>
-      <c r="B114" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="C114" s="10" t="s">
+      <c r="B114" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C114" s="7" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="9">
+      <c r="A115" s="25">
         <v>43470499</v>
       </c>
-      <c r="B115" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="C115" s="10" t="s">
+      <c r="B115" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C115" s="7" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="9">
+      <c r="A116" s="25">
         <v>800060288</v>
       </c>
-      <c r="B116" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="C116" s="10" t="s">
+      <c r="B116" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C116" s="7" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="9">
+      <c r="A117" s="25">
         <v>901731328</v>
       </c>
-      <c r="B117" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="C117" s="10" t="s">
+      <c r="B117" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C117" s="7" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="9">
+      <c r="A118" s="25">
         <v>890903939</v>
       </c>
-      <c r="B118" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="C118" s="10" t="s">
+      <c r="B118" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C118" s="7" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="9">
+      <c r="A119" s="25">
         <v>900162861</v>
       </c>
-      <c r="B119" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="C119" s="10" t="s">
+      <c r="B119" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="9">
+      <c r="A120" s="25">
         <v>891303109</v>
       </c>
-      <c r="B120" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="C120" s="10" t="s">
+      <c r="B120" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C120" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="9">
+      <c r="A121" s="25">
         <v>817002753</v>
       </c>
-      <c r="B121" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="C121" s="10" t="s">
+      <c r="B121" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C121" s="7" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="9">
+      <c r="A122" s="25">
         <v>901238919</v>
       </c>
-      <c r="B122" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="C122" s="10" t="s">
+      <c r="B122" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C122" s="7" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="9">
+      <c r="A123" s="25">
         <v>1040732318</v>
       </c>
-      <c r="B123" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="C123" s="10" t="s">
+      <c r="B123" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C123" s="7" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="9">
+      <c r="A124" s="25">
         <v>811006146</v>
       </c>
-      <c r="B124" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="C124" s="10" t="s">
+      <c r="B124" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C124" s="7" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="9">
+      <c r="A125" s="25">
         <v>71690934</v>
       </c>
-      <c r="B125" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="C125" s="10" t="s">
+      <c r="B125" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C125" s="7" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="9">
+      <c r="A126" s="25">
         <v>901218826</v>
       </c>
-      <c r="B126" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="C126" s="10" t="s">
+      <c r="B126" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C126" s="7" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="9">
+      <c r="A127" s="25">
         <v>900316481</v>
       </c>
-      <c r="B127" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="C127" s="10" t="s">
+      <c r="B127" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="9">
+      <c r="A128" s="25">
         <v>800197463</v>
       </c>
-      <c r="B128" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="C128" s="10" t="s">
+      <c r="B128" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C128" s="7" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="9">
+      <c r="A129" s="25">
         <v>900483321</v>
       </c>
-      <c r="B129" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="C129" s="10" t="s">
+      <c r="B129" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C129" s="7" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="9">
+      <c r="A130" s="25">
         <v>70692652</v>
       </c>
-      <c r="B130" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="C130" s="10" t="s">
+      <c r="B130" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C130" s="7" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="9">
+      <c r="A131" s="25">
         <v>901017416</v>
       </c>
-      <c r="B131" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="C131" s="10" t="s">
+      <c r="B131" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C131" s="7" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="9">
+      <c r="A132" s="25">
         <v>890903253</v>
       </c>
-      <c r="B132" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="C132" s="10" t="s">
+      <c r="B132" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C132" s="7" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="9">
+      <c r="A133" s="25">
         <v>860004922</v>
       </c>
-      <c r="B133" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="C133" s="10" t="s">
+      <c r="B133" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C133" s="7" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="9">
+      <c r="A134" s="25">
         <v>900336556</v>
       </c>
-      <c r="B134" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="C134" s="10" t="s">
+      <c r="B134" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C134" s="7" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="9">
+      <c r="A135" s="25">
         <v>890935900</v>
       </c>
-      <c r="B135" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="C135" s="10" t="s">
+      <c r="B135" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C135" s="7" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="9">
+      <c r="A136" s="25">
         <v>811022302</v>
       </c>
-      <c r="B136" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="C136" s="10" t="s">
+      <c r="B136" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C136" s="7" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="9">
+      <c r="A137" s="25">
         <v>900806261</v>
       </c>
-      <c r="B137" s="24" t="s">
-        <v>313</v>
-      </c>
-      <c r="C137" s="10" t="s">
+      <c r="B137" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="C137" s="7" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="22">
+      <c r="A138" s="30">
         <v>900279378</v>
       </c>
-      <c r="B138" s="25" t="s">
-        <v>314</v>
-      </c>
-      <c r="C138" s="23" t="s">
+      <c r="B138" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="C138" s="12" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="9">
+      <c r="A139" s="25">
         <v>900810414</v>
       </c>
-      <c r="B139" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="C139" s="10" t="s">
+      <c r="B139" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C139" s="7" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="9">
+      <c r="A140" s="25">
         <v>800143643</v>
       </c>
-      <c r="B140" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="C140" s="10" t="s">
+      <c r="B140" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C140" s="7" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="15">
+      <c r="A141" s="27">
         <v>900916161</v>
       </c>
-      <c r="B141" s="16" t="s">
-        <v>317</v>
-      </c>
-      <c r="C141" s="16" t="s">
+      <c r="B141" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="C141" s="9" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="15">
+      <c r="A142" s="27">
         <v>891201294</v>
       </c>
-      <c r="B142" s="16" t="s">
-        <v>318</v>
-      </c>
-      <c r="C142" s="16" t="s">
+      <c r="B142" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="C142" s="9" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="18">
+      <c r="A143" s="28">
         <v>890907797</v>
       </c>
-      <c r="B143" s="19" t="s">
-        <v>319</v>
-      </c>
-      <c r="C143" s="19" t="s">
+      <c r="B143" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="C143" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="15">
+      <c r="A144" s="27">
         <v>830514992</v>
       </c>
-      <c r="B144" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="C144" s="16" t="s">
+      <c r="B144" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="C144" s="9" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="15">
+      <c r="A145" s="27">
         <v>890914979</v>
       </c>
-      <c r="B145" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="C145" s="16" t="s">
+      <c r="B145" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="C145" s="9" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="26">
+      <c r="A146" s="31">
         <v>900937354</v>
       </c>
-      <c r="B146" s="27" t="s">
-        <v>322</v>
-      </c>
-      <c r="C146" s="27" t="s">
+      <c r="B146" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="C146" s="15" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="28">
+      <c r="A147" s="32">
         <v>901827068</v>
       </c>
-      <c r="B147" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="C147" s="29" t="s">
+      <c r="B147" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="C147" s="16" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="26">
+      <c r="A148" s="31">
         <v>1039447150</v>
       </c>
-      <c r="B148" s="27" t="s">
-        <v>324</v>
-      </c>
-      <c r="C148" s="27" t="s">
+      <c r="B148" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C148" s="15" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="12">
+      <c r="A149" s="26">
         <v>900741033</v>
       </c>
-      <c r="B149" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="C149" s="13" t="s">
+      <c r="B149" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C149" s="8" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="9">
+      <c r="A150" s="25">
         <v>800186960</v>
       </c>
-      <c r="B150" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="C150" s="10" t="s">
+      <c r="B150" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C150" s="7" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="9">
+      <c r="A151" s="25">
         <v>80018696</v>
       </c>
-      <c r="B151" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="C151" s="10" t="s">
+      <c r="B151" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C151" s="7" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="9">
+      <c r="A152" s="25">
         <v>800186960</v>
       </c>
-      <c r="B152" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="C152" s="10" t="s">
+      <c r="B152" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C152" s="7" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="9">
+      <c r="A153" s="25">
         <v>800186960</v>
       </c>
-      <c r="B153" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="C153" s="10" t="s">
+      <c r="B153" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C153" s="7" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="26">
+      <c r="A154" s="31">
         <v>71600395</v>
       </c>
-      <c r="B154" s="27" t="s">
+      <c r="B154" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="C154" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="28">
+        <v>900488269</v>
+      </c>
+      <c r="B155" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="C155" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="27">
+        <v>900804607</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="27">
+        <v>860000258</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="27">
+        <v>890916575</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="27">
+        <v>890903858</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="27">
+        <v>811003604</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="27">
+        <v>900821440</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="27">
+        <v>800004228</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="C162" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="28">
+        <v>820003519</v>
+      </c>
+      <c r="B163" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C163" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="27">
+        <v>800186960</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="C164" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="29">
+        <v>900559359</v>
+      </c>
+      <c r="B165" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="C165" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="25">
+        <v>800186960</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C166" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="27">
+        <v>890937015</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="27">
+        <v>890201881</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C168" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="28">
+        <v>901177226</v>
+      </c>
+      <c r="B169" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="C169" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="27">
+        <v>901122735</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="29">
+        <v>901528790</v>
+      </c>
+      <c r="B171" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C171" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="25">
+        <v>800186960</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C172" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="25">
+        <v>800186960</v>
+      </c>
+      <c r="B173" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="C154" s="27" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="18">
-        <v>900488269</v>
-      </c>
-      <c r="B155" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="C155" s="19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="15">
-        <v>900804607</v>
-      </c>
-      <c r="B156" s="16" t="s">
-        <v>331</v>
-      </c>
-      <c r="C156" s="16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="15">
-        <v>860000258</v>
-      </c>
-      <c r="B157" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="C157" s="16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="15">
-        <v>890916575</v>
-      </c>
-      <c r="B158" s="16" t="s">
-        <v>333</v>
-      </c>
-      <c r="C158" s="16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="15">
-        <v>890903858</v>
-      </c>
-      <c r="B159" s="16" t="s">
-        <v>334</v>
-      </c>
-      <c r="C159" s="16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="15">
-        <v>811003604</v>
-      </c>
-      <c r="B160" s="16" t="s">
-        <v>335</v>
-      </c>
-      <c r="C160" s="16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="15">
-        <v>900821440</v>
-      </c>
-      <c r="B161" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="C161" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="15">
-        <v>800004228</v>
-      </c>
-      <c r="B162" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="C162" s="16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="18">
-        <v>820003519</v>
-      </c>
-      <c r="B163" s="19" t="s">
-        <v>338</v>
-      </c>
-      <c r="C163" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="15">
+      <c r="C173" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="25">
         <v>800186960</v>
       </c>
-      <c r="B164" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="C164" s="16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="20">
-        <v>900559359</v>
-      </c>
-      <c r="B165" s="21" t="s">
-        <v>339</v>
-      </c>
-      <c r="C165" s="21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="9">
+      <c r="B174" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="25">
         <v>800186960</v>
       </c>
-      <c r="B166" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="C166" s="10" t="s">
+      <c r="B175" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C175" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="15">
-        <v>890937015</v>
-      </c>
-      <c r="B167" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="C167" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="15">
-        <v>890201881</v>
-      </c>
-      <c r="B168" s="16" t="s">
-        <v>341</v>
-      </c>
-      <c r="C168" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="18">
-        <v>901177226</v>
-      </c>
-      <c r="B169" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="C169" s="19" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="15">
-        <v>901122735</v>
-      </c>
-      <c r="B170" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="C170" s="16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="20">
-        <v>901528790</v>
-      </c>
-      <c r="B171" s="21" t="s">
-        <v>344</v>
-      </c>
-      <c r="C171" s="21" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="9">
-        <v>800186960</v>
-      </c>
-      <c r="B172" s="10" t="s">
-        <v>345</v>
-      </c>
-      <c r="C172" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="9">
-        <v>800186960</v>
-      </c>
-      <c r="B173" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="C173" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="9">
-        <v>800186960</v>
-      </c>
-      <c r="B174" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="C174" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="9">
-        <v>800186960</v>
-      </c>
-      <c r="B175" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="C175" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
     <row r="176" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="20">
+      <c r="A176" s="29">
         <v>901287954</v>
       </c>
-      <c r="B176" s="21" t="s">
-        <v>348</v>
-      </c>
-      <c r="C176" s="21" t="s">
+      <c r="B176" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="C176" s="11" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="9">
+      <c r="A177" s="25">
         <v>890904478</v>
       </c>
-      <c r="B177" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="C177" s="10" t="s">
+      <c r="B177" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C177" s="7" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="26">
+      <c r="A178" s="31">
         <v>890904478</v>
       </c>
-      <c r="B178" s="27" t="s">
-        <v>350</v>
-      </c>
-      <c r="C178" s="27" t="s">
+      <c r="B178" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="C178" s="15" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="28">
+      <c r="A179" s="32">
         <v>890101676</v>
       </c>
-      <c r="B179" s="29" t="s">
-        <v>351</v>
-      </c>
-      <c r="C179" s="29" t="s">
+      <c r="B179" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="C179" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="26">
+      <c r="A180" s="31">
         <v>811010574</v>
       </c>
-      <c r="B180" s="27" t="s">
-        <v>352</v>
-      </c>
-      <c r="C180" s="27" t="s">
+      <c r="B180" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C180" s="15" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="28">
+      <c r="A181" s="32">
         <v>890301163</v>
       </c>
-      <c r="B181" s="29" t="s">
-        <v>353</v>
-      </c>
-      <c r="C181" s="29" t="s">
+      <c r="B181" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="C181" s="16" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="26">
+      <c r="A182" s="31">
         <v>890301163</v>
       </c>
-      <c r="B182" s="27" t="s">
-        <v>354</v>
-      </c>
-      <c r="C182" s="27" t="s">
+      <c r="B182" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="C182" s="15" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="28">
+      <c r="A183" s="32">
         <v>8568191</v>
       </c>
-      <c r="B183" s="29" t="s">
-        <v>355</v>
-      </c>
-      <c r="C183" s="29" t="s">
+      <c r="B183" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="C183" s="16" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="26">
+      <c r="A184" s="31">
         <v>900467839</v>
       </c>
-      <c r="B184" s="27" t="s">
-        <v>356</v>
-      </c>
-      <c r="C184" s="27" t="s">
+      <c r="B184" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="C184" s="15" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="28">
+      <c r="A185" s="32">
         <v>800197463</v>
       </c>
-      <c r="B185" s="29" t="s">
-        <v>357</v>
-      </c>
-      <c r="C185" s="29" t="s">
+      <c r="B185" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="C185" s="16" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="30">
+      <c r="A186" s="31">
         <v>860000135</v>
       </c>
-      <c r="B186" s="31" t="s">
-        <v>358</v>
-      </c>
-      <c r="C186" s="31" t="s">
+      <c r="B186" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="C186" s="15" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="32"/>
-      <c r="B187" s="32"/>
-      <c r="C187" s="32"/>
+      <c r="A187" s="32">
+        <v>891100445</v>
+      </c>
+      <c r="B187" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="C187" s="16" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="188" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="32"/>
-      <c r="B188" s="32"/>
-      <c r="C188" s="32"/>
+      <c r="A188" s="31">
+        <v>890300466</v>
+      </c>
+      <c r="B188" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="C188" s="15" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="189" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="32"/>
-      <c r="B189" s="32"/>
-      <c r="C189" s="32"/>
+      <c r="A189" s="33">
+        <v>900929629</v>
+      </c>
+      <c r="B189" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="C189" s="17" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="190" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="32"/>
-      <c r="B190" s="32"/>
-      <c r="C190" s="32"/>
+      <c r="A190" s="18"/>
+      <c r="B190" s="18"/>
+      <c r="C190" s="18"/>
     </row>
     <row r="191" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="32"/>
-      <c r="B191" s="32"/>
-      <c r="C191" s="32"/>
+      <c r="A191" s="18"/>
+      <c r="B191" s="18"/>
+      <c r="C191" s="18"/>
     </row>
     <row r="192" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="32"/>
-      <c r="C192" s="32"/>
+      <c r="A192" s="18"/>
+      <c r="B192" s="18"/>
+      <c r="C192" s="3"/>
     </row>
     <row r="193" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="32"/>
+      <c r="A193" s="18"/>
     </row>
     <row r="194" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="32"/>
+      <c r="A194" s="18"/>
     </row>
     <row r="195" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="32"/>
+      <c r="A195" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B112" r:id="rId1" xr:uid="{A31211B8-BF9B-45F5-B606-5097A0DA1E0A}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>